<commit_message>
fix null value exception
</commit_message>
<xml_diff>
--- a/kpiExcelSheet/nhóm L3.xlsx
+++ b/kpiExcelSheet/nhóm L3.xlsx
@@ -511,7 +511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -693,27 +693,32 @@
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
-          <t>Hoàn thành đúng tiến độ và chất lượng các Công việc phát sinh/ Seminar/ Cải tiến</t>
+          <t xml:space="preserve">Đảm bảo chất lượng sản phẩm 
+1. PTSP: với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK, SmartRouting
+2. Vận hành: Đảm bảo cam kết thời gian khắc phục lỗi từ lúc phát hiện đến khi xử lý xong
+</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>Tổ chức Seminar các công nghệ, xu hướng trên thị trường v.v … nhằm gia tăng hiểu biết của một nhóm nhân sự</t>
+          <t>Đảm bảo chất lượng sản phẩm với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK, SmartRouting</t>
         </is>
       </c>
       <c r="D4" s="8" t="inlineStr">
         <is>
-          <t>Hoàn thành xây dựng template log format và triển khai tích hợp ELK cho các dự án SOP trước 23.08.2023</t>
+          <t>Trên môi trường stg Trung bình số bugs cá nhân và team được report trong mỗi tính năng khi review code/ thực hiện dev &lt;= 5 và trên môi trường UAT và production có critical/important issue &lt;= 1</t>
         </is>
       </c>
       <c r="E4" s="8" t="inlineStr">
         <is>
-          <t>Báo cáo được CBQL confirm</t>
+          <t>- STG: số bug/tính năng khi review code/ thực hiện dev &lt;= 5
+- UAT/PROD: critical/important issue &lt;= 1 và lỗi lặp = 0
+** Không tính issue do nguyên nhân enhancement, wishlist, support</t>
         </is>
       </c>
       <c r="F4" s="8" t="inlineStr">
         <is>
-          <t>Mail</t>
+          <t>Taiga</t>
         </is>
       </c>
       <c r="G4" s="8" t="inlineStr">
@@ -723,7 +728,7 @@
       </c>
       <c r="H4" s="8" t="inlineStr">
         <is>
-          <t>Đạt/Không đạt</t>
+          <t>%</t>
         </is>
       </c>
       <c r="I4" s="8" t="inlineStr">
@@ -733,29 +738,25 @@
       </c>
       <c r="J4" s="8" t="inlineStr">
         <is>
-          <t>Đạt</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="K4" s="8" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L4" s="8" t="n">
         <v>100</v>
       </c>
       <c r="M4" s="8" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N4" s="8" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="O4" s="8" t="n">
-        <v>31</v>
-      </c>
-      <c r="P4" s="8" t="inlineStr">
-        <is>
-          <t>'- Xây dựng template, tích hợp vào source code: 2h/tuần = 8h/tháng</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P4" s="8" t="n"/>
       <c r="Q4" s="8" t="inlineStr">
         <is>
           <r>
@@ -768,7 +769,7 @@
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">https://drive.google.com/file/d/1Pbtci9OOtsXW1xbX5YOWNKKpJFwQ8W3X/view?usp=sharing
+            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/12xRR9qnXMPQwbbMVJNh_tgojw_33x8ItlEbBmNyfmlI/edit?usp=sharing
 </t>
           </r>
         </is>
@@ -779,30 +780,30 @@
       <c r="A5" s="2" t="n"/>
       <c r="B5" s="8" t="inlineStr">
         <is>
-          <t>Đảm bảo chất lượng sản phẩm với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK</t>
+          <t xml:space="preserve">Đảm bảo chất lượng sản phẩm 
+1. PTSP: với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK, SmartRouting
+2. Vận hành: Đảm bảo cam kết thời gian khắc phục lỗi từ lúc phát hiện đến khi xử lý xong
+</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>Đảm bảo chất lượng và trách nhiệm với số bug được kiểm soát trong dự án SOP</t>
+          <t>Tỷ lệ cam kết thời gian khắc phục lỗi từ lúc phát hiện đến khi xử lý xong &gt;= 90%</t>
         </is>
       </c>
       <c r="D5" s="8" t="inlineStr">
         <is>
-          <t>Trên môi trường stg Trung bình số bugs cá nhân và team được report trong mỗi tính năng khi review code/ thực hiện dev &lt;= 5 và trên môi trường UAT critical/important issue &lt;= 1</t>
+          <t>Tỷ lệ hoàn thành xử lý lỗi vận hành đúng hạn &gt;= 90%</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>Đảm bảo số bug cá nhân và team thỏa:
-- STG: số bug/tính năng khi review code/ thực hiện dev &lt;= 5
-- UAT: critical/important issue &lt;= 1
-** Không tính issue do nguyên nhân enhancement, wishlist, support</t>
+          <t>Tổng số ticket đúng hạn trong tháng/ Tổng số ticket nhận trong tháng</t>
         </is>
       </c>
       <c r="F5" s="8" t="inlineStr">
         <is>
-          <t>Taiga</t>
+          <t>Mail</t>
         </is>
       </c>
       <c r="G5" s="8" t="inlineStr">
@@ -826,38 +827,34 @@
         </is>
       </c>
       <c r="K5" s="8" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="L5" s="8" t="n">
         <v>100</v>
       </c>
       <c r="M5" s="8" t="n">
-        <v/>
+        <v>0</v>
       </c>
       <c r="N5" s="8" t="n">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="O5" s="8" t="n">
-        <v>20</v>
-      </c>
-      <c r="P5" s="8" t="inlineStr">
-        <is>
-          <t>Reivew bugs, tìm giải pháp: 1h/ngày = 23h/tháng</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="P5" s="8" t="n"/>
       <c r="Q5" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">Thống kê bugs : </t>
+            <t xml:space="preserve">Bằng chứng : </t>
           </r>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1zYsbMX-Gft2b4pZZdDyLumB5I78fhNHAE3t62baPN6s/edit?usp=sharing
+            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/12xRR9qnXMPQwbbMVJNh_tgojw_33x8ItlEbBmNyfmlI/edit?usp=sharing
 </t>
           </r>
         </is>
@@ -865,253 +862,273 @@
       <c r="R5" s="8" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="B6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="C6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="D6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="E6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="F6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="G6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="J6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="K6" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="L6" s="9" t="n">
-        <v>200</v>
-      </c>
-      <c r="M6" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="9" t="inlineStr"/>
-      <c r="O6" s="9" t="inlineStr"/>
-      <c r="P6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="Q6" s="8" t="n">
-        <v/>
-      </c>
-      <c r="R6" s="8" t="n">
-        <v/>
-      </c>
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="8" t="inlineStr">
+        <is>
+          <t>Hoàn thành đúng tiến độ và chất lượng các Công việc phát sinh/ Seminar/ Cải tiến</t>
+        </is>
+      </c>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>Tổ chức Seminar các công nghệ, xu hướng trên thị trường v.v … nhằm gia tăng hiểu biết của một nhóm nhân sự</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Hoàn thành xây dựng quy trình thi Olympic, xét chức danh và bộ đề thi cho phòng RnD trước 23.09.2023</t>
+        </is>
+      </c>
+      <c r="E6" s="8" t="inlineStr">
+        <is>
+          <t>Báo cáo được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>Mail</t>
+        </is>
+      </c>
+      <c r="G6" s="8" t="inlineStr">
+        <is>
+          <t>Tháng</t>
+        </is>
+      </c>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I6" s="8" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="J6" s="8" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="K6" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="n">
+        <v>66</v>
+      </c>
+      <c r="M6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="8" t="n">
+        <v>24</v>
+      </c>
+      <c r="O6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="8" t="n"/>
+      <c r="Q6" s="8" t="n"/>
+      <c r="R6" s="8" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="A7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="B7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="K7" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" s="9" t="n">
+        <v>266</v>
+      </c>
+      <c r="M7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="9" t="inlineStr"/>
+      <c r="O7" s="9" t="inlineStr"/>
+      <c r="P7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="Q7" s="8" t="n">
+        <v/>
+      </c>
+      <c r="R7" s="8" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
         <is>
           <t>okr</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Nâng cao chất lượng hoàn thành phát triển và release 100% các tính năng trong dự án trung tâm OnCX, SOP, HappyConnect, Dialo, CheckMK đúng thời hạn cam kết</t>
         </is>
       </c>
-      <c r="C7" s="8" t="inlineStr">
-        <is>
-          <t>Hoàn thành release các tính năng bản web và apps theo kế hoạch trong tháng 8</t>
-        </is>
-      </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>Hoàn thành release các tính năng bản web và apps theo kế hoạch trong tháng 9</t>
+        </is>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>Đảm bảo 100% các tính năng trong sprint được giao hoàn thành đúng thời hạn (dự án SOP)</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
-        <is>
-          <t>100% US/ sprint hoàn thành thỏa cả 2 điều kiện:
+      <c r="E8" s="8" t="inlineStr">
+        <is>
+          <t>'SOP
+100% US/ sprint hoàn thành thỏa cả 3 điều kiện:
 - Có bằng chứng dev intergration test/ unittest ở mt dev
-- Tester test pass các US trên mt stg</t>
-        </is>
-      </c>
-      <c r="F7" s="8" t="inlineStr">
+- Tester test pass các US trên mt stg
+- Release đúng tiến độ tính năng được phân công</t>
+        </is>
+      </c>
+      <c r="F8" s="8" t="inlineStr">
         <is>
           <t>Taiga</t>
         </is>
       </c>
-      <c r="G7" s="8" t="inlineStr">
+      <c r="G8" s="8" t="inlineStr">
         <is>
           <t>Tháng</t>
         </is>
       </c>
-      <c r="H7" s="8" t="inlineStr">
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="I7" s="8" t="inlineStr">
+      <c r="I8" s="8" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="J7" s="8" t="inlineStr">
+      <c r="J8" s="8" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
       </c>
-      <c r="K7" s="8" t="n">
+      <c r="K8" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="L7" s="8" t="n">
-        <v>92</v>
-      </c>
-      <c r="M7" s="8" t="n">
-        <v/>
-      </c>
-      <c r="N7" s="8" t="n">
-        <v>147</v>
-      </c>
-      <c r="O7" s="8" t="n">
+      <c r="L8" s="8" t="n">
+        <v>81</v>
+      </c>
+      <c r="M8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="8" t="n">
         <v>116</v>
       </c>
-      <c r="P7" s="8" t="inlineStr">
-        <is>
-          <t>- Review code: 1h/ngày = 23h/tháng
-- Meeting daily SOP 0.5h/ngày = 11.5h/tháng
-- Meeting retro, review, planning : 6h SOP/sprint = 12h/tháng
-- Code tính năng 4h/ngày = 92h/tháng
-- Làm báo cáo và thực hiện báo cáo: 2h/tuần = 8h/tháng</t>
-        </is>
-      </c>
-      <c r="Q7" s="8" t="inlineStr">
+      <c r="O8" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8" t="n"/>
+      <c r="Q8" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">Tiến độ SOP SP20 : </t>
+            <t xml:space="preserve">Bằng chứng : </t>
           </r>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1JxytDSIKmv1RNPyIQ0Ocwn1-zJwOdqS4aWsx-ZNBl5o/edit?usp=sharing
+            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/12xRR9qnXMPQwbbMVJNh_tgojw_33x8ItlEbBmNyfmlI/edit?usp=sharing
 </t>
           </r>
         </is>
       </c>
-      <c r="R7" s="8" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="B8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="C8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="D8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="E8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="F8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="J8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="K8" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="L8" s="9" t="n">
-        <v>92</v>
-      </c>
-      <c r="M8" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="9" t="n">
-        <v>184</v>
-      </c>
-      <c r="O8" s="9" t="n">
-        <v>167</v>
-      </c>
-      <c r="P8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="Q8" s="8" t="n">
-        <v/>
-      </c>
-      <c r="R8" s="8" t="n">
-        <v/>
-      </c>
+      <c r="R8" s="8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="n"/>
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n"/>
-      <c r="E9" s="2" t="n"/>
-      <c r="F9" s="2" t="n"/>
-      <c r="G9" s="2" t="n"/>
-      <c r="H9" s="2" t="n"/>
-      <c r="I9" s="2" t="n"/>
-      <c r="J9" s="2" t="n"/>
-      <c r="K9" s="2" t="n"/>
-      <c r="L9" s="2" t="n"/>
-      <c r="M9" s="2" t="n"/>
-      <c r="N9" s="2" t="n"/>
-      <c r="O9" s="2" t="n"/>
-      <c r="P9" s="2" t="n"/>
-      <c r="Q9" s="2" t="n"/>
-      <c r="R9" s="2" t="n"/>
+      <c r="A9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="B9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="K9" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" s="9" t="n">
+        <v>81</v>
+      </c>
+      <c r="M9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9" t="n">
+        <v>170</v>
+      </c>
+      <c r="O9" s="9" t="inlineStr"/>
+      <c r="P9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="Q9" s="8" t="n">
+        <v/>
+      </c>
+      <c r="R9" s="8" t="n">
+        <v/>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="inlineStr">
-        <is>
-          <t>Trương Tấn Sang</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="inlineStr">
-        <is>
-          <t>sangtt9</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="inlineStr">
-        <is>
-          <t>L3</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
-        <is>
-          <t>Team FE</t>
-        </is>
-      </c>
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="2" t="n"/>
+      <c r="D10" s="2" t="n"/>
+      <c r="E10" s="2" t="n"/>
       <c r="F10" s="2" t="n"/>
       <c r="G10" s="2" t="n"/>
       <c r="H10" s="2" t="n"/>
@@ -1127,427 +1144,376 @@
       <c r="R10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Loại</t>
-        </is>
-      </c>
-      <c r="B11" s="5" t="inlineStr">
-        <is>
-          <t>KR phòng</t>
-        </is>
-      </c>
-      <c r="C11" s="5" t="inlineStr">
-        <is>
-          <t>KR team</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="inlineStr">
-        <is>
-          <t>KR cá nhân</t>
-        </is>
-      </c>
-      <c r="E11" s="5" t="inlineStr">
-        <is>
-          <t>Công thức tính</t>
-        </is>
-      </c>
-      <c r="F11" s="5" t="inlineStr">
-        <is>
-          <t>Nguồn dữ liệu</t>
-        </is>
-      </c>
-      <c r="G11" s="5" t="inlineStr">
-        <is>
-          <t>Định kỳ tính</t>
-        </is>
-      </c>
-      <c r="H11" s="5" t="inlineStr">
-        <is>
-          <t>Đơn vị tính</t>
-        </is>
-      </c>
-      <c r="I11" s="5" t="inlineStr">
-        <is>
-          <t>Điều kiện</t>
-        </is>
-      </c>
-      <c r="J11" s="5" t="inlineStr">
-        <is>
-          <t>Norm</t>
-        </is>
-      </c>
-      <c r="K11" s="6" t="inlineStr">
-        <is>
-          <t>% Trọng số chỉ tiêu</t>
-        </is>
-      </c>
-      <c r="L11" s="6" t="inlineStr">
-        <is>
-          <t>Kết quả</t>
-        </is>
-      </c>
-      <c r="M11" s="6" t="inlineStr">
-        <is>
-          <t>Tỷ lệ</t>
-        </is>
-      </c>
-      <c r="N11" s="6" t="inlineStr">
-        <is>
-          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
-        </is>
-      </c>
-      <c r="O11" s="4" t="inlineStr">
-        <is>
-          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
-        </is>
-      </c>
-      <c r="P11" s="6" t="inlineStr">
-        <is>
-          <t>Note dự kiến</t>
-        </is>
-      </c>
-      <c r="Q11" s="4" t="inlineStr">
-        <is>
-          <t>Note bằng chứng thực tế</t>
-        </is>
-      </c>
-      <c r="R11" s="7" t="inlineStr">
-        <is>
-          <t>QA</t>
-        </is>
-      </c>
+      <c r="A11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Trương Tấn Sang</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>sangtt9</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>L3</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>Team FE</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
+      <c r="H11" s="2" t="n"/>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="2" t="n"/>
+      <c r="K11" s="2" t="n"/>
+      <c r="L11" s="2" t="n"/>
+      <c r="M11" s="2" t="n"/>
+      <c r="N11" s="2" t="n"/>
+      <c r="O11" s="2" t="n"/>
+      <c r="P11" s="2" t="n"/>
+      <c r="Q11" s="2" t="n"/>
+      <c r="R11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Loại</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>KR phòng</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>KR team</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>KR cá nhân</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>Công thức tính</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>Nguồn dữ liệu</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>Định kỳ tính</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>Đơn vị tính</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>Điều kiện</t>
+        </is>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t>Norm</t>
+        </is>
+      </c>
+      <c r="K12" s="6" t="inlineStr">
+        <is>
+          <t>% Trọng số chỉ tiêu</t>
+        </is>
+      </c>
+      <c r="L12" s="6" t="inlineStr">
+        <is>
+          <t>Kết quả</t>
+        </is>
+      </c>
+      <c r="M12" s="6" t="inlineStr">
+        <is>
+          <t>Tỷ lệ</t>
+        </is>
+      </c>
+      <c r="N12" s="6" t="inlineStr">
+        <is>
+          <t>Tổng thời gian dự kiến/ ước tính công việc (giờ)</t>
+        </is>
+      </c>
+      <c r="O12" s="4" t="inlineStr">
+        <is>
+          <t>Tổng thời gian thực hiện công việc thực tế (giờ)</t>
+        </is>
+      </c>
+      <c r="P12" s="6" t="inlineStr">
+        <is>
+          <t>Note dự kiến</t>
+        </is>
+      </c>
+      <c r="Q12" s="4" t="inlineStr">
+        <is>
+          <t>Note bằng chứng thực tế</t>
+        </is>
+      </c>
+      <c r="R12" s="7" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="inlineStr">
         <is>
           <t>kpi</t>
         </is>
       </c>
-      <c r="B12" s="8" t="inlineStr">
-        <is>
-          <t>Đảm bảo chất lượng sản phẩm với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK</t>
-        </is>
-      </c>
-      <c r="C12" s="8" t="inlineStr">
-        <is>
-          <t>Đảm bảo chất lượng sản phẩm với số bug log trên các môi trường trong dự án OnCX, SOP</t>
-        </is>
-      </c>
-      <c r="D12" s="8" t="inlineStr">
-        <is>
-          <t>Trên môi trường stg Trung bình số bugs cá nhân và team được report trong mỗi tính năng khi review code/ thực hiện dev &lt;= 5 và trên môi trường UAT critical/important issue &lt;= 1</t>
-        </is>
-      </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
+        <is>
+          <t>Hoàn thành đúng tiến độ và chất lượng các Công việc phát sinh/ Seminar/ Cải tiến</t>
+        </is>
+      </c>
+      <c r="C13" s="8" t="inlineStr">
+        <is>
+          <t>Đảm bảo các công việc phát sinh hoàn thành đúng tiến độ và chất lượng</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
+        <is>
+          <t>- Hoàn thành xây dựng bộ đề thi xét duyệt chức danh và nội dung ôn tập cho nhân sự cho phòng RnD trước 23.09.2023.</t>
+        </is>
+      </c>
+      <c r="E13" s="8" t="inlineStr">
+        <is>
+          <t>Báo cáo bộ đề được CBQL confirm</t>
+        </is>
+      </c>
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>Mail</t>
+        </is>
+      </c>
+      <c r="G13" s="8" t="inlineStr">
+        <is>
+          <t>Tháng</t>
+        </is>
+      </c>
+      <c r="H13" s="8" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I13" s="8" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="F12" s="8" t="inlineStr">
+      <c r="J13" s="8" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="K13" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8" t="n"/>
+      <c r="Q13" s="8" t="n"/>
+      <c r="R13" s="8" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n"/>
+      <c r="B14" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Đảm bảo chất lượng sản phẩm 
+1. PTSP: với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK, SmartRouting
+2. Vận hành: Đảm bảo cam kết thời gian khắc phục lỗi từ lúc phát hiện đến khi xử lý xong
+</t>
+        </is>
+      </c>
+      <c r="C14" s="8" t="inlineStr">
+        <is>
+          <t>Tỷ lệ cam kết thời gian khắc phục lỗi từ lúc phát hiện đến khi xử lý xong &gt;= 90%</t>
+        </is>
+      </c>
+      <c r="D14" s="8" t="inlineStr">
+        <is>
+          <t>Tỷ lệ hoàn thành xử lý lỗi vận hành đúng hạn &gt;= 90%</t>
+        </is>
+      </c>
+      <c r="E14" s="8" t="inlineStr">
+        <is>
+          <t>Tổng số ticket đúng hạn trong tháng/ Tổng số ticket nhận trong tháng</t>
+        </is>
+      </c>
+      <c r="F14" s="8" t="inlineStr">
         <is>
           <t>Taiga</t>
         </is>
       </c>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="G14" s="8" t="inlineStr">
         <is>
           <t>Tháng</t>
         </is>
       </c>
-      <c r="H12" s="8" t="inlineStr">
+      <c r="H14" s="8" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="I12" s="8" t="inlineStr">
+      <c r="I14" s="8" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="J12" s="8" t="inlineStr">
+      <c r="J14" s="8" t="inlineStr">
         <is>
           <t>100%</t>
         </is>
       </c>
-      <c r="K12" s="8" t="n">
-        <v>70</v>
-      </c>
-      <c r="L12" s="8" t="n">
+      <c r="K14" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="L14" s="8" t="n">
         <v>100</v>
       </c>
-      <c r="M12" s="8" t="n">
-        <v/>
-      </c>
-      <c r="N12" s="8" t="n">
-        <v>36</v>
-      </c>
-      <c r="O12" s="8" t="n">
-        <v>16</v>
-      </c>
-      <c r="P12" s="8" t="inlineStr">
-        <is>
-          <t>OnCX: review merge code, họp 10h/tháng
-SOP: review merge code, fix issue 26h/tháng</t>
-        </is>
-      </c>
-      <c r="Q12" s="8" t="inlineStr">
+      <c r="M14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="8" t="n"/>
+      <c r="Q14" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">Bằng chứng SOP : </t>
+            <t xml:space="preserve">Bằng chứng : </t>
           </r>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1RhypsQkAzhg2KbmyNZK4cuOIm6D9OEHNzGXMOfb_1bY/edit?usp=sharing
+            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/12xRR9qnXMPQwbbMVJNh_tgojw_33x8ItlEbBmNyfmlI/edit?usp=sharing
 </t>
           </r>
+        </is>
+      </c>
+      <c r="R14" s="8" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n"/>
+      <c r="B15" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Đảm bảo chất lượng sản phẩm 
+1. PTSP: với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK, SmartRouting
+2. Vận hành: Đảm bảo cam kết thời gian khắc phục lỗi từ lúc phát hiện đến khi xử lý xong
+</t>
+        </is>
+      </c>
+      <c r="C15" s="8" t="inlineStr">
+        <is>
+          <t>Đảm bảo chất lượng sản phẩm với số bug log trên các môi trường trong dự án OnCX, SOP, HappyConnect, Dialo, CheckMK, SmartRouting</t>
+        </is>
+      </c>
+      <c r="D15" s="8" t="inlineStr">
+        <is>
+          <t>Trên môi trường stg Trung bình số bugs cá nhân và team được report trong mỗi tính năng khi review code/ thực hiện dev &lt;= 5 và trên môi trường UAT và production có critical/important issue &lt;= 1</t>
+        </is>
+      </c>
+      <c r="E15" s="8" t="inlineStr">
+        <is>
+          <t>- STG: số bug/tính năng khi review code/ thực hiện dev &lt;= 5
+- UAT/PROD: critical/important issue &lt;= 1 và lỗi lặp = 0
+** Không tính issue do nguyên nhân enhancement, wishlist, support</t>
+        </is>
+      </c>
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>Taiga</t>
+        </is>
+      </c>
+      <c r="G15" s="8" t="inlineStr">
+        <is>
+          <t>Tháng</t>
+        </is>
+      </c>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I15" s="8" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="J15" s="8" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="K15" s="8" t="n">
+        <v>40</v>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="M15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="8" t="inlineStr">
+        <is>
+          <t>OnCX: review merge code, họp 5h/tháng
+SOP: review merge code, fix issue 25h/tháng</t>
+        </is>
+      </c>
+      <c r="Q15" s="8" t="inlineStr">
+        <is>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">Bằng chứng OnCX : </t>
+            <t xml:space="preserve">Bằng chứng : </t>
           </r>
           <r>
             <rPr>
               <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
             </rPr>
-            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1DLjc-lC8n9fdbc0kWZ_C_Q_PUNAVQPv7/edit?usp=sharing&amp;ouid=109873007904207433989&amp;rtpof=true&amp;sd=true
-</t>
-          </r>
-        </is>
-      </c>
-      <c r="R12" s="8" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n"/>
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>Hoàn thành đúng tiến độ và chất lượng các Công việc phát sinh/ Seminar/ Cải tiến</t>
-        </is>
-      </c>
-      <c r="C13" s="8" t="inlineStr">
-        <is>
-          <t>Đảm bảo các công việc phát sinh hoàn thành đúng tiến độ và chất lượng</t>
-        </is>
-      </c>
-      <c r="D13" s="8" t="inlineStr">
-        <is>
-          <t>Áp dụng lowcode notification và import file OKR KPI lên Tool nhân sự trước 23.8.2023</t>
-        </is>
-      </c>
-      <c r="E13" s="8" t="inlineStr">
-        <is>
-          <t>Báo cáo được CBQL confirm</t>
-        </is>
-      </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>Mail</t>
-        </is>
-      </c>
-      <c r="G13" s="8" t="inlineStr">
-        <is>
-          <t>Tháng</t>
-        </is>
-      </c>
-      <c r="H13" s="8" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="I13" s="8" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
-      <c r="J13" s="8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="K13" s="8" t="n">
-        <v>30</v>
-      </c>
-      <c r="L13" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="8" t="n">
-        <v/>
-      </c>
-      <c r="N13" s="8" t="n">
-        <v>76</v>
-      </c>
-      <c r="O13" s="8" t="n">
-        <v>96</v>
-      </c>
-      <c r="P13" s="8" t="inlineStr">
-        <is>
-          <t>- Triển khai lowcode notification: 16h
-- Áp dụng low import file OKR, KPI: 32h</t>
-        </is>
-      </c>
-      <c r="Q13" s="8" t="n"/>
-      <c r="R13" s="8" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="B14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="C14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="D14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="E14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="F14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="G14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="I14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="J14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="K14" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="L14" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="M14" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" s="9" t="inlineStr"/>
-      <c r="O14" s="9" t="inlineStr"/>
-      <c r="P14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="Q14" s="8" t="n">
-        <v/>
-      </c>
-      <c r="R14" s="8" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="inlineStr">
-        <is>
-          <t>okr</t>
-        </is>
-      </c>
-      <c r="B15" s="8" t="inlineStr">
-        <is>
-          <t>Nâng cao chất lượng hoàn thành phát triển và release 100% các tính năng trong dự án trung tâm OnCX, SOP, HappyConnect, Dialo, CheckMK đúng thời hạn cam kết</t>
-        </is>
-      </c>
-      <c r="C15" s="8" t="inlineStr">
-        <is>
-          <t>Hoàn thành release các tính năng bản apps v1.1, release các tính năng theo kế hoạch trong tháng 8</t>
-        </is>
-      </c>
-      <c r="D15" s="8" t="inlineStr">
-        <is>
-          <t>Đảm bảo 100% các tính năng trong sprint được giao hoàn thành đúng thời hạn (dự án SOP, OnCX)</t>
-        </is>
-      </c>
-      <c r="E15" s="8" t="inlineStr">
-        <is>
-          <t>100% US/ sprint hoàn thành thỏa cả 2 điều kiện:
-- Có bằng chứng dev intergration test/ unittest ở mt dev
-- Tester test pass các US trên mt stg</t>
-        </is>
-      </c>
-      <c r="F15" s="8" t="inlineStr">
-        <is>
-          <t>Taiga</t>
-        </is>
-      </c>
-      <c r="G15" s="8" t="inlineStr">
-        <is>
-          <t>Tháng</t>
-        </is>
-      </c>
-      <c r="H15" s="8" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="I15" s="8" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
-      <c r="J15" s="8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="K15" s="8" t="n">
-        <v>100</v>
-      </c>
-      <c r="L15" s="8" t="n">
-        <v>96</v>
-      </c>
-      <c r="M15" s="8" t="n">
-        <v/>
-      </c>
-      <c r="N15" s="8" t="n">
-        <v>72</v>
-      </c>
-      <c r="O15" s="8" t="n">
-        <v>62</v>
-      </c>
-      <c r="P15" s="8" t="inlineStr">
-        <is>
-          <t>SOP:
-- Daily SOP: 0.5h/ngày * 19 = 9.5h/tháng
-- Sprint planing - retro review: 8h/tháng
-- Báo cáo report tuần: 2h/tháng
-- Thực hiện task: 14h/tháng</t>
-        </is>
-      </c>
-      <c r="Q15" s="8" t="inlineStr">
-        <is>
-          <r>
-            <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
-            </rPr>
-            <t xml:space="preserve">Bằng chứng SOP : </t>
-          </r>
-          <r>
-            <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
-            </rPr>
-            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1JxytDSIKmv1RNPyIQ0Ocwn1-zJwOdqS4aWsx-ZNBl5o/edit?usp=sharing
-</t>
-          </r>
-          <r>
-            <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='00FF0000', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
-            </rPr>
-            <t xml:space="preserve">Bằng chứng OnCX : </t>
-          </r>
-          <r>
-            <rPr>
-              <rFont val="&lt;openpyxl.styles.fonts.Font object&gt;&#10;Parameters:&#10;name='Arial', charset=None, family=None, b=False, i=False, strike=False, outline=None, shadow=None, condense=None, color=&lt;openpyxl.styles.colors.Color object&gt;&#10;Parameters:&#10;rgb='006699CC', indexed=None, auto=None, theme=None, tint=0.0, type='rgb', extend=None, sz=11.0, u=None, vertAlign=None, scheme=None"/>
-            </rPr>
-            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/1DLjc-lC8n9fdbc0kWZ_C_Q_PUNAVQPv7/edit?usp=sharing&amp;ouid=109873007904207433989&amp;rtpof=true&amp;sd=true
+            <t xml:space="preserve">https://docs.google.com/spreadsheets/d/12xRR9qnXMPQwbbMVJNh_tgojw_33x8ItlEbBmNyfmlI/edit?usp=sharing
 </t>
           </r>
         </is>
@@ -1589,17 +1555,13 @@
         <v>100</v>
       </c>
       <c r="L16" s="9" t="n">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="M16" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="N16" s="9" t="n">
-        <v>184</v>
-      </c>
-      <c r="O16" s="9" t="n">
-        <v>174</v>
-      </c>
+      <c r="N16" s="9" t="inlineStr"/>
+      <c r="O16" s="9" t="inlineStr"/>
       <c r="P16" s="8" t="n">
         <v/>
       </c>
@@ -1607,16 +1569,146 @@
         <v/>
       </c>
       <c r="R16" s="8" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>okr</t>
+        </is>
+      </c>
+      <c r="B17" s="8" t="inlineStr">
+        <is>
+          <t>Nâng cao chất lượng hoàn thành phát triển và release 100% các tính năng trong dự án trung tâm OnCX, SOP, HappyConnect, Dialo, CheckMK đúng thời hạn cam kết</t>
+        </is>
+      </c>
+      <c r="C17" s="8" t="inlineStr">
+        <is>
+          <t>Hoàn thành release các tính năng bản apps v1.1, release các tính năng theo kế hoạch trong tháng 9</t>
+        </is>
+      </c>
+      <c r="D17" s="8" t="inlineStr">
+        <is>
+          <t>- Đảm bảo 100% các tính năng trong sprint được giao hoàn thành đúng thời hạn (dự án SOP, OnCX, ChatbotAI)</t>
+        </is>
+      </c>
+      <c r="E17" s="8" t="inlineStr">
+        <is>
+          <t>1. SOP/OnCX
+100% US/ sprint hoàn thành thỏa cả 3 điều kiện:
+- Có bằng chứng dev intergration test/ unittest ở mt dev
+- Tester test pass các US trên mt stg
+- Release đúng tiến độ tính năng được phân công
+2. ChatbotAI
+- Kế hoạch/ bài toán + metrics chatbot cho VH được BGĐ confirm</t>
+        </is>
+      </c>
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>Taiga</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="inlineStr">
+        <is>
+          <t>Tháng</t>
+        </is>
+      </c>
+      <c r="H17" s="8" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="I17" s="8" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="J17" s="8" t="inlineStr">
+        <is>
+          <t>100%</t>
+        </is>
+      </c>
+      <c r="K17" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="L17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>98</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="8" t="n"/>
+      <c r="Q17" s="8" t="n"/>
+      <c r="R17" s="8" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="B18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="E18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="H18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="I18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="J18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="K18" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="L18" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="9" t="n">
+        <v>128</v>
+      </c>
+      <c r="O18" s="9" t="inlineStr"/>
+      <c r="P18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="Q18" s="8" t="n">
+        <v/>
+      </c>
+      <c r="R18" s="8" t="n">
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A15"/>
-    <mergeCell ref="A7"/>
+    <mergeCell ref="A8"/>
+    <mergeCell ref="A17"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>